<commit_message>
Updates comp_benchmarking_comparison.xlsx with pangenome size comparison
</commit_message>
<xml_diff>
--- a/data/computation_benchmarking/comp_benchmarking_comparison.xlsx
+++ b/data/computation_benchmarking/comp_benchmarking_comparison.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sth19\PycharmProjects\PhD_project\ggCaller_manuscript\data\computation_benchmarking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4AA1EA-6908-4E85-A1DB-5E6A26ADBB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0401ABE7-6251-4A5C-8C52-FC0B69A79D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29670" yWindow="2130" windowWidth="21600" windowHeight="11325" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="graph_complexity_pneumo" sheetId="5" r:id="rId1"/>
     <sheet name="benchmark_pneumo" sheetId="8" r:id="rId2"/>
+    <sheet name="Pangenome_size" sheetId="9" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="35">
   <si>
     <t>Tool</t>
   </si>
@@ -124,6 +125,24 @@
   </si>
   <si>
     <t>V+E</t>
+  </si>
+  <si>
+    <t>Panaroo</t>
+  </si>
+  <si>
+    <t>PEPPAN</t>
+  </si>
+  <si>
+    <t>Roary</t>
+  </si>
+  <si>
+    <t>No. Core COGs</t>
+  </si>
+  <si>
+    <t>No. Total COGs</t>
+  </si>
+  <si>
+    <t>No. Accessory COGs</t>
   </si>
 </sst>
 </file>
@@ -1233,7 +1252,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ABABA53-DDA6-4703-98FC-E7BB0090EDD5}">
   <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -4055,4 +4074,1871 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66B0BF1-30FB-4F10-A076-1A55A8BF2CB3}">
+  <dimension ref="A1:G77"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>1724</v>
+      </c>
+      <c r="F2">
+        <v>2427</v>
+      </c>
+      <c r="G2">
+        <f>F2-E2</f>
+        <v>703</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>1625</v>
+      </c>
+      <c r="F3">
+        <v>3005</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G66" si="0">F3-E3</f>
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
+      <c r="E4">
+        <v>1508</v>
+      </c>
+      <c r="F4">
+        <v>3992</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>2484</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5">
+        <v>100</v>
+      </c>
+      <c r="E5">
+        <v>1526</v>
+      </c>
+      <c r="F5">
+        <v>4637</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>3111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6">
+        <v>500</v>
+      </c>
+      <c r="E6">
+        <v>1472</v>
+      </c>
+      <c r="F6">
+        <v>6037</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>4565</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7">
+        <v>1000</v>
+      </c>
+      <c r="E7">
+        <v>1466</v>
+      </c>
+      <c r="F7">
+        <v>6766</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>5300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8">
+        <v>2000</v>
+      </c>
+      <c r="E8">
+        <v>1462</v>
+      </c>
+      <c r="F8">
+        <v>7833</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>6371</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>1720</v>
+      </c>
+      <c r="F9">
+        <v>2379</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>659</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>1577</v>
+      </c>
+      <c r="F10">
+        <v>2859</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11">
+        <v>50</v>
+      </c>
+      <c r="E11">
+        <v>1510</v>
+      </c>
+      <c r="F11">
+        <v>3610</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12">
+        <v>1499</v>
+      </c>
+      <c r="F12">
+        <v>3836</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>2337</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13">
+        <v>500</v>
+      </c>
+      <c r="E13">
+        <v>1518</v>
+      </c>
+      <c r="F13">
+        <v>4358</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>2840</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>1898</v>
+      </c>
+      <c r="F14">
+        <v>2258</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <v>1876</v>
+      </c>
+      <c r="F15">
+        <v>2276</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16">
+        <v>50</v>
+      </c>
+      <c r="E16">
+        <v>492</v>
+      </c>
+      <c r="F16">
+        <v>2550</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>2058</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17">
+        <v>100</v>
+      </c>
+      <c r="E17">
+        <v>1770</v>
+      </c>
+      <c r="F17">
+        <v>2556</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>786</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18">
+        <v>500</v>
+      </c>
+      <c r="E18">
+        <v>1797</v>
+      </c>
+      <c r="F18">
+        <v>3874</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>2077</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19">
+        <v>1000</v>
+      </c>
+      <c r="E19">
+        <v>1816</v>
+      </c>
+      <c r="F19">
+        <v>6319</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>4503</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20">
+        <v>3000</v>
+      </c>
+      <c r="E20">
+        <v>1885</v>
+      </c>
+      <c r="F20">
+        <v>11757</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>9872</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>1688</v>
+      </c>
+      <c r="F21">
+        <v>2409</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>721</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22">
+        <v>10</v>
+      </c>
+      <c r="E22">
+        <v>1594</v>
+      </c>
+      <c r="F22">
+        <v>2946</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23">
+        <v>50</v>
+      </c>
+      <c r="E23">
+        <v>1496</v>
+      </c>
+      <c r="F23">
+        <v>4014</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>2518</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24">
+        <v>100</v>
+      </c>
+      <c r="E24">
+        <v>1494</v>
+      </c>
+      <c r="F24">
+        <v>4649</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>3155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25">
+        <v>500</v>
+      </c>
+      <c r="E25">
+        <v>1433</v>
+      </c>
+      <c r="F25">
+        <v>5952</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>4519</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26">
+        <v>1000</v>
+      </c>
+      <c r="E26">
+        <v>1399</v>
+      </c>
+      <c r="F26">
+        <v>6585</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>5186</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27">
+        <v>2000</v>
+      </c>
+      <c r="E27">
+        <v>1361</v>
+      </c>
+      <c r="F27">
+        <v>7620</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>6259</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <v>1685</v>
+      </c>
+      <c r="F28">
+        <v>2340</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>655</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29">
+        <v>10</v>
+      </c>
+      <c r="E29">
+        <v>1554</v>
+      </c>
+      <c r="F29">
+        <v>2797</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30">
+        <v>50</v>
+      </c>
+      <c r="E30">
+        <v>1515</v>
+      </c>
+      <c r="F30">
+        <v>3186</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31">
+        <v>100</v>
+      </c>
+      <c r="E31">
+        <v>1497</v>
+      </c>
+      <c r="F31">
+        <v>3476</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32">
+        <v>500</v>
+      </c>
+      <c r="E32">
+        <v>1497</v>
+      </c>
+      <c r="F32">
+        <v>3872</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>2375</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33">
+        <v>5</v>
+      </c>
+      <c r="E33">
+        <v>1878</v>
+      </c>
+      <c r="F33">
+        <v>2256</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>378</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34">
+        <v>10</v>
+      </c>
+      <c r="E34">
+        <v>1857</v>
+      </c>
+      <c r="F34">
+        <v>2255</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="0"/>
+        <v>398</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35">
+        <v>50</v>
+      </c>
+      <c r="E35">
+        <v>289</v>
+      </c>
+      <c r="F35">
+        <v>2391</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="0"/>
+        <v>2102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36">
+        <v>100</v>
+      </c>
+      <c r="E36">
+        <v>1728</v>
+      </c>
+      <c r="F36">
+        <v>2445</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="0"/>
+        <v>717</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37">
+        <v>500</v>
+      </c>
+      <c r="E37">
+        <v>1703</v>
+      </c>
+      <c r="F37">
+        <v>2566</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="0"/>
+        <v>863</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38">
+        <v>1000</v>
+      </c>
+      <c r="E38">
+        <v>1667</v>
+      </c>
+      <c r="F38">
+        <v>3877</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="0"/>
+        <v>2210</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39">
+        <v>3000</v>
+      </c>
+      <c r="E39">
+        <v>1642</v>
+      </c>
+      <c r="F39">
+        <v>7991</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="0"/>
+        <v>6349</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40">
+        <v>5</v>
+      </c>
+      <c r="E40">
+        <v>1703</v>
+      </c>
+      <c r="F40">
+        <v>2547</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="0"/>
+        <v>844</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41">
+        <v>10</v>
+      </c>
+      <c r="E41">
+        <v>1611</v>
+      </c>
+      <c r="F41">
+        <v>3235</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="0"/>
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42">
+        <v>50</v>
+      </c>
+      <c r="E42">
+        <v>1519</v>
+      </c>
+      <c r="F42">
+        <v>4444</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="0"/>
+        <v>2925</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43">
+        <v>100</v>
+      </c>
+      <c r="E43">
+        <v>1431</v>
+      </c>
+      <c r="F43">
+        <v>5113</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="0"/>
+        <v>3682</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44">
+        <v>500</v>
+      </c>
+      <c r="E44">
+        <v>1260</v>
+      </c>
+      <c r="F44">
+        <v>7212</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="0"/>
+        <v>5952</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>30</v>
+      </c>
+      <c r="B45" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45">
+        <v>1000</v>
+      </c>
+      <c r="E45">
+        <v>1171</v>
+      </c>
+      <c r="F45">
+        <v>8767</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="0"/>
+        <v>7596</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46">
+        <v>2000</v>
+      </c>
+      <c r="E46" t="s">
+        <v>27</v>
+      </c>
+      <c r="F46" t="s">
+        <v>27</v>
+      </c>
+      <c r="G46" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>30</v>
+      </c>
+      <c r="B47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" t="s">
+        <v>24</v>
+      </c>
+      <c r="D47">
+        <v>5</v>
+      </c>
+      <c r="E47">
+        <v>1721</v>
+      </c>
+      <c r="F47">
+        <v>2442</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="0"/>
+        <v>721</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>30</v>
+      </c>
+      <c r="B48" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48">
+        <v>10</v>
+      </c>
+      <c r="E48">
+        <v>1598</v>
+      </c>
+      <c r="F48">
+        <v>2996</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="0"/>
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>30</v>
+      </c>
+      <c r="B49" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" t="s">
+        <v>24</v>
+      </c>
+      <c r="D49">
+        <v>50</v>
+      </c>
+      <c r="E49">
+        <v>1542</v>
+      </c>
+      <c r="F49">
+        <v>3611</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="0"/>
+        <v>2069</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>30</v>
+      </c>
+      <c r="B50" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" t="s">
+        <v>24</v>
+      </c>
+      <c r="D50">
+        <v>100</v>
+      </c>
+      <c r="E50">
+        <v>1483</v>
+      </c>
+      <c r="F50">
+        <v>3814</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="0"/>
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>30</v>
+      </c>
+      <c r="B51" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" t="s">
+        <v>24</v>
+      </c>
+      <c r="D51">
+        <v>500</v>
+      </c>
+      <c r="E51">
+        <v>1422</v>
+      </c>
+      <c r="F51">
+        <v>4452</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="0"/>
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>30</v>
+      </c>
+      <c r="B52" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" t="s">
+        <v>25</v>
+      </c>
+      <c r="D52">
+        <v>5</v>
+      </c>
+      <c r="E52">
+        <v>1910</v>
+      </c>
+      <c r="F52">
+        <v>2271</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="0"/>
+        <v>361</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>30</v>
+      </c>
+      <c r="B53" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" t="s">
+        <v>25</v>
+      </c>
+      <c r="D53">
+        <v>10</v>
+      </c>
+      <c r="E53">
+        <v>1883</v>
+      </c>
+      <c r="F53">
+        <v>2314</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="0"/>
+        <v>431</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>30</v>
+      </c>
+      <c r="B54" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" t="s">
+        <v>25</v>
+      </c>
+      <c r="D54">
+        <v>50</v>
+      </c>
+      <c r="E54">
+        <v>1618</v>
+      </c>
+      <c r="F54">
+        <v>5191</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="0"/>
+        <v>3573</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>30</v>
+      </c>
+      <c r="B55" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" t="s">
+        <v>25</v>
+      </c>
+      <c r="D55">
+        <v>100</v>
+      </c>
+      <c r="E55">
+        <v>1603</v>
+      </c>
+      <c r="F55">
+        <v>5310</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="0"/>
+        <v>3707</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>30</v>
+      </c>
+      <c r="B56" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" t="s">
+        <v>25</v>
+      </c>
+      <c r="D56">
+        <v>500</v>
+      </c>
+      <c r="E56">
+        <v>1549</v>
+      </c>
+      <c r="F56">
+        <v>13344</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="0"/>
+        <v>11795</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>30</v>
+      </c>
+      <c r="B57" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" t="s">
+        <v>25</v>
+      </c>
+      <c r="D57">
+        <v>1000</v>
+      </c>
+      <c r="E57">
+        <v>1521</v>
+      </c>
+      <c r="F57">
+        <v>23587</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="0"/>
+        <v>22066</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>30</v>
+      </c>
+      <c r="B58" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" t="s">
+        <v>25</v>
+      </c>
+      <c r="D58">
+        <v>3000</v>
+      </c>
+      <c r="E58">
+        <v>192</v>
+      </c>
+      <c r="F58">
+        <v>47872</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="0"/>
+        <v>47680</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>31</v>
+      </c>
+      <c r="B59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s">
+        <v>23</v>
+      </c>
+      <c r="D59">
+        <v>5</v>
+      </c>
+      <c r="E59">
+        <v>1543</v>
+      </c>
+      <c r="F59">
+        <v>2881</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="0"/>
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>31</v>
+      </c>
+      <c r="B60" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60">
+        <v>10</v>
+      </c>
+      <c r="E60">
+        <v>1438</v>
+      </c>
+      <c r="F60">
+        <v>3760</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="0"/>
+        <v>2322</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>31</v>
+      </c>
+      <c r="B61" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" t="s">
+        <v>23</v>
+      </c>
+      <c r="D61">
+        <v>50</v>
+      </c>
+      <c r="E61">
+        <v>1250</v>
+      </c>
+      <c r="F61">
+        <v>6040</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="0"/>
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>31</v>
+      </c>
+      <c r="B62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" t="s">
+        <v>23</v>
+      </c>
+      <c r="D62">
+        <v>100</v>
+      </c>
+      <c r="E62">
+        <v>1222</v>
+      </c>
+      <c r="F62">
+        <v>7360</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="0"/>
+        <v>6138</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>31</v>
+      </c>
+      <c r="B63" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" t="s">
+        <v>23</v>
+      </c>
+      <c r="D63">
+        <v>500</v>
+      </c>
+      <c r="E63">
+        <v>965</v>
+      </c>
+      <c r="F63">
+        <v>12189</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="0"/>
+        <v>11224</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" t="s">
+        <v>23</v>
+      </c>
+      <c r="D64">
+        <v>1000</v>
+      </c>
+      <c r="E64">
+        <v>848</v>
+      </c>
+      <c r="F64">
+        <v>15187</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="0"/>
+        <v>14339</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>31</v>
+      </c>
+      <c r="B65" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" t="s">
+        <v>23</v>
+      </c>
+      <c r="D65">
+        <v>2000</v>
+      </c>
+      <c r="E65">
+        <v>697</v>
+      </c>
+      <c r="F65">
+        <v>19354</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="0"/>
+        <v>18657</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>31</v>
+      </c>
+      <c r="B66" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" t="s">
+        <v>24</v>
+      </c>
+      <c r="D66">
+        <v>5</v>
+      </c>
+      <c r="E66">
+        <v>1553</v>
+      </c>
+      <c r="F66">
+        <v>2773</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="0"/>
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>31</v>
+      </c>
+      <c r="B67" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" t="s">
+        <v>24</v>
+      </c>
+      <c r="D67">
+        <v>10</v>
+      </c>
+      <c r="E67">
+        <v>1381</v>
+      </c>
+      <c r="F67">
+        <v>3655</v>
+      </c>
+      <c r="G67">
+        <f t="shared" ref="G67:G77" si="1">F67-E67</f>
+        <v>2274</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>31</v>
+      </c>
+      <c r="B68" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" t="s">
+        <v>24</v>
+      </c>
+      <c r="D68">
+        <v>50</v>
+      </c>
+      <c r="E68">
+        <v>1302</v>
+      </c>
+      <c r="F68">
+        <v>4719</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="1"/>
+        <v>3417</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B69" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" t="s">
+        <v>24</v>
+      </c>
+      <c r="D69">
+        <v>100</v>
+      </c>
+      <c r="E69">
+        <v>1256</v>
+      </c>
+      <c r="F69">
+        <v>5333</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="1"/>
+        <v>4077</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>31</v>
+      </c>
+      <c r="B70" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" t="s">
+        <v>24</v>
+      </c>
+      <c r="D70">
+        <v>500</v>
+      </c>
+      <c r="E70">
+        <v>1164</v>
+      </c>
+      <c r="F70">
+        <v>7133</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="1"/>
+        <v>5969</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>31</v>
+      </c>
+      <c r="B71" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" t="s">
+        <v>25</v>
+      </c>
+      <c r="D71">
+        <v>5</v>
+      </c>
+      <c r="E71">
+        <v>1785</v>
+      </c>
+      <c r="F71">
+        <v>2516</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="1"/>
+        <v>731</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>31</v>
+      </c>
+      <c r="B72" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" t="s">
+        <v>25</v>
+      </c>
+      <c r="D72">
+        <v>10</v>
+      </c>
+      <c r="E72">
+        <v>1751</v>
+      </c>
+      <c r="F72">
+        <v>2642</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="1"/>
+        <v>891</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>31</v>
+      </c>
+      <c r="B73" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" t="s">
+        <v>25</v>
+      </c>
+      <c r="D73">
+        <v>50</v>
+      </c>
+      <c r="E73">
+        <v>689</v>
+      </c>
+      <c r="F73">
+        <v>8288</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="1"/>
+        <v>7599</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>31</v>
+      </c>
+      <c r="B74" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" t="s">
+        <v>25</v>
+      </c>
+      <c r="D74">
+        <v>100</v>
+      </c>
+      <c r="E74">
+        <v>1385</v>
+      </c>
+      <c r="F74">
+        <v>8781</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="1"/>
+        <v>7396</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>31</v>
+      </c>
+      <c r="B75" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" t="s">
+        <v>25</v>
+      </c>
+      <c r="D75">
+        <v>500</v>
+      </c>
+      <c r="E75">
+        <v>1451</v>
+      </c>
+      <c r="F75">
+        <v>18644</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="1"/>
+        <v>17193</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>31</v>
+      </c>
+      <c r="B76" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" t="s">
+        <v>25</v>
+      </c>
+      <c r="D76">
+        <v>1000</v>
+      </c>
+      <c r="E76">
+        <v>1393</v>
+      </c>
+      <c r="F76">
+        <v>30952</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="1"/>
+        <v>29559</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>31</v>
+      </c>
+      <c r="B77" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" t="s">
+        <v>25</v>
+      </c>
+      <c r="D77">
+        <v>3000</v>
+      </c>
+      <c r="E77">
+        <v>1240</v>
+      </c>
+      <c r="F77">
+        <v>63615</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="1"/>
+        <v>62375</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>